<commit_message>
Added more tests for registration page
</commit_message>
<xml_diff>
--- a/ToolsQA/ToolsQA.Tests/TestData/UserData.xlsx
+++ b/ToolsQA/ToolsQA.Tests/TestData/UserData.xlsx
@@ -81,9 +81,6 @@
     <t>Single</t>
   </si>
   <si>
-    <t>WirhoutCountry</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>WithoutCountry</t>
   </si>
 </sst>
 </file>
@@ -415,7 +415,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -528,12 +528,12 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -545,10 +545,10 @@
         <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1">
         <v>33406</v>

</xml_diff>